<commit_message>
Add Bird and in Bonus U as referencedTileType
</commit_message>
<xml_diff>
--- a/level.xlsx
+++ b/level.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Java\FlappyBird\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucie\Desktop\Java\FlappyBird\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="8">
   <si>
     <t>W</t>
   </si>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -366,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG17"/>
+  <dimension ref="A1:AK17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z18" sqref="Z18"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,12 +377,12 @@
     <col min="1" max="38" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -405,7 +405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -428,7 +428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -474,7 +474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -494,7 +494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
@@ -502,7 +502,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="I8" t="s">
         <v>0</v>
       </c>
@@ -521,8 +521,11 @@
       <c r="AG8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AK8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="I9" t="s">
         <v>0</v>
       </c>
@@ -542,10 +545,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="I10" t="s">
         <v>0</v>
       </c>
+      <c r="K10" t="s">
+        <v>5</v>
+      </c>
       <c r="P10" t="s">
         <v>0</v>
       </c>
@@ -561,32 +567,47 @@
       <c r="AG10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="P11" t="s">
         <v>0</v>
       </c>
+      <c r="Y11" t="s">
+        <v>5</v>
+      </c>
       <c r="AC11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="P12" t="s">
         <v>0</v>
       </c>
+      <c r="S12" t="s">
+        <v>5</v>
+      </c>
       <c r="AC12" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AK12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="L13" t="s">
         <v>0</v>
       </c>
       <c r="Y13" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AK13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="L14" t="s">
         <v>0</v>
       </c>
@@ -599,8 +620,11 @@
       <c r="AG14" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AK14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="I15" t="s">
         <v>0</v>
       </c>
@@ -622,8 +646,11 @@
       <c r="AG15" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AK15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="I16" t="s">
         <v>0</v>
       </c>
@@ -651,8 +678,11 @@
       <c r="AG16" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AK16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -750,6 +780,18 @@
         <v>2</v>
       </c>
       <c r="AG17" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK17" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>